<commit_message>
Torque Magnético - Terminado
</commit_message>
<xml_diff>
--- a/Magnetic Torque/Data/Precession.xlsx
+++ b/Magnetic Torque/Data/Precession.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Laboratorio_Intermedio\Magnetic Torque\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3782391-77AE-4C25-A619-7CD974AC6381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C9DB9E-CFA2-4202-87C6-D1A8B0163239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{A1CD7762-1091-46DD-B282-7CF36D3E4DF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A1CD7762-1091-46DD-B282-7CF36D3E4DF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Current [A]</t>
   </si>
   <si>
     <t>Period [s] (4.5 Hz)</t>
+  </si>
+  <si>
+    <t>Period [s] (5 Hz)</t>
+  </si>
+  <si>
+    <t>Period [s] (6 Hz)</t>
   </si>
 </sst>
 </file>
@@ -416,7 +422,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,10 +440,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -544,6 +550,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5efcfc4f-29bb-494d-9a76-b0329a59025e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001FC1E8C1DD8F5B41A47A8ECFEE6084B1" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="362953927954337d30e3444b1491acb4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5efcfc4f-29bb-494d-9a76-b0329a59025e" xmlns:ns4="35d47d0e-5fff-46fc-9dc4-f42efd9cfec7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="45be33ed40e230c63a3ad38fd1900dda" ns3:_="" ns4:_="">
     <xsd:import namespace="5efcfc4f-29bb-494d-9a76-b0329a59025e"/>
@@ -776,24 +799,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5efcfc4f-29bb-494d-9a76-b0329a59025e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{168264AB-BEA6-4031-945C-A54E70544708}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5efcfc4f-29bb-494d-9a76-b0329a59025e"/>
+    <ds:schemaRef ds:uri="35d47d0e-5fff-46fc-9dc4-f42efd9cfec7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BAD5E3C-9CFA-424F-A819-F10CE5E9B184}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{292B3A03-FF95-48EC-A9C7-9725E4138E9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -810,29 +841,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BAD5E3C-9CFA-424F-A819-F10CE5E9B184}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{168264AB-BEA6-4031-945C-A54E70544708}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5efcfc4f-29bb-494d-9a76-b0329a59025e"/>
-    <ds:schemaRef ds:uri="35d47d0e-5fff-46fc-9dc4-f42efd9cfec7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>